<commit_message>
Saved codes and links data\
</commit_message>
<xml_diff>
--- a/src/test/resources/codes_links.xlsx
+++ b/src/test/resources/codes_links.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t xml:space="preserve">PROMO CODE</t>
   </si>
@@ -62,6 +62,18 @@
   </si>
   <si>
     <t>https://amzn.to/3kQbTa8</t>
+  </si>
+  <si>
+    <t>69226XKI</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2GphbKL</t>
+  </si>
+  <si>
+    <t>5049YPD2</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3enAIYD</t>
   </si>
 </sst>
 </file>
@@ -260,42 +272,42 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>